<commit_message>
add styles to home app and update tour app
</commit_message>
<xml_diff>
--- a/instance/tours.xlsx
+++ b/instance/tours.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dlitdp-my.sharepoint.com/personal/kavunenko_y_dlit_dp_ua/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crazy\Downloads\Telegram Desktop\дз лицей 2024\Flask_Tour\instance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{F3A181BE-1DC8-4725-95ED-205AE5E2BAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4557FF8F-3230-4DB0-8285-6A3D7B0CDB93}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EB9DD5-10F8-43F0-97D1-46BAAF81B1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0191FA6F-903A-4157-A2BF-B6C98CBE7969}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,20 +767,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0f42d56c-4d91-40f0-a2b7-8244c6f15481" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0f42d56c-4d91-40f0-a2b7-8244c6f15481" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,14 +803,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D89EABC-4137-4209-AA0C-D14E48274401}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73FB273C-899C-4704-875C-A0E6321243A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -825,4 +817,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D89EABC-4137-4209-AA0C-D14E48274401}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>